<commit_message>
Automatización con usuarios obtenidos desde data driven, lee usuarios y escribe estado de autenticación
</commit_message>
<xml_diff>
--- a/datadrivenlogin.xlsx
+++ b/datadrivenlogin.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Hoja 1" r:id="rId3" sheetId="1" state="visible"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -33,11 +35,18 @@
   <si>
     <t>xxxxxxxx</t>
   </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -63,29 +72,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -109,6 +118,9 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -116,6 +128,9 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -125,6 +140,9 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -133,6 +151,9 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Test Pinterest e Instagram
</commit_message>
<xml_diff>
--- a/datadrivenlogin.xlsx
+++ b/datadrivenlogin.xlsx
@@ -1,19 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView activeTab="0"/>
-  </bookViews>
   <sheets>
-    <sheet name="Hoja 1" r:id="rId3" sheetId="1" state="visible"/>
+    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -30,30 +28,38 @@
     <t>medellin</t>
   </si>
   <si>
+    <t>uditeamacn1@gmail.com</t>
+  </si>
+  <si>
+    <t>Medellin20171</t>
+  </si>
+  <si>
     <t>zzzzzzzz</t>
   </si>
   <si>
+    <t>xxxxxxxxx</t>
+  </si>
+  <si>
     <t>pavasmarcela</t>
   </si>
   <si>
     <t>simpsons</t>
   </si>
   <si>
+    <t>marcela.pavas@gmail.com</t>
+  </si>
+  <si>
     <t>xxxxxxxx</t>
   </si>
   <si>
-    <t>Correct</t>
-  </si>
-  <si>
-    <t>Incorrect</t>
+    <t>Medellin2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <numFmts count="0"/>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -61,34 +67,8 @@
     </font>
     <font/>
     <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,35 +88,32 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -160,8 +137,11 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -169,32 +149,41 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -204,8 +193,11 @@
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatizaciòn Completa Pinterest e Instagram
</commit_message>
<xml_diff>
--- a/datadrivenlogin.xlsx
+++ b/datadrivenlogin.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Hoja 1" r:id="rId3" sheetId="1" state="visible"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -53,13 +55,26 @@
   </si>
   <si>
     <t>Medellin2017</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <numFmts count="0"/>
+  <fonts count="16">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -69,6 +84,64 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,32 +161,45 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="16">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment/>
     </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -137,11 +223,17 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -157,6 +249,9 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -171,6 +266,9 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -185,6 +283,9 @@
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -193,11 +294,17 @@
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>